<commit_message>
Added : Implemented profile page
</commit_message>
<xml_diff>
--- a/PageObjectModel/src/main/resources/repository/LoginTestData.xlsx
+++ b/PageObjectModel/src/main/resources/repository/LoginTestData.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\eclipse-workspace\PageObjectModel\src\main\resources\repository\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84E0DE2B-3603-4176-85A4-2AAC7849A4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B1BD63FE-1DB6-4447-8147-FF320846A07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="888" windowWidth="17280" windowHeight="8964" xr2:uid="{C103208C-5D0B-4325-B206-98DE625BC3BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C103208C-5D0B-4325-B206-98DE625BC3BE}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,13 +37,13 @@
     <t>password</t>
   </si>
   <si>
-    <t>sonar.mayuresh260197@gmail.com</t>
-  </si>
-  <si>
     <t>Test@12345</t>
   </si>
   <si>
     <t>Test@1234567458</t>
+  </si>
+  <si>
+    <t>kumarbob912@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -413,7 +409,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,26 +428,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{9DFE6FAE-C1E2-4104-86D0-2EEF5CC578FC}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{54AD7410-FEEE-4387-8BF4-CA3174050DA5}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{CC05EBA6-11AE-4C3F-914F-0C7B78C39975}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{BA71AD57-4825-4E0A-80E7-2B123A0ACA24}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{54AD7410-FEEE-4387-8BF4-CA3174050DA5}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{BA71AD57-4825-4E0A-80E7-2B123A0ACA24}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{E14C991A-85BD-4804-BE7B-4FCB300012CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>